<commit_message>
Index Constitiuents - return % combined
</commit_message>
<xml_diff>
--- a/returnPct/returns.xlsx
+++ b/returnPct/returns.xlsx
@@ -474,65 +474,65 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>^CNXPSUBANK</t>
+          <t>^ENGINEERING</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7015.5</v>
+        <v>8509.219999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>8378.7001953125</v>
+        <v>10155.62</v>
       </c>
       <c r="D3" t="n">
-        <v>19.43126213830091</v>
+        <v>19.34842441492876</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>^ENGINEERING</t>
+          <t>^MOTORFINANCE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8509.18</v>
+        <v>47571.16</v>
       </c>
       <c r="C4" t="n">
-        <v>10057.23</v>
+        <v>56441.72</v>
       </c>
       <c r="D4" t="n">
-        <v>18.19270481997089</v>
+        <v>18.64692809677123</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M%26M.NS</t>
+          <t>^CNXPSUBANK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3177.76953125</v>
+        <v>7015.5</v>
       </c>
       <c r="C5" t="n">
-        <v>3749.60009765625</v>
+        <v>8253.2001953125</v>
       </c>
       <c r="D5" t="n">
-        <v>17.99471487100942</v>
+        <v>17.64236612233626</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>^MOTORFINANCE</t>
+          <t>^CONVENTIONAL2AND3WHEELERS</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>47571.29</v>
+        <v>64297.09</v>
       </c>
       <c r="C6" t="n">
-        <v>55517.21</v>
+        <v>74536.62</v>
       </c>
       <c r="D6" t="n">
-        <v>16.70318379005488</v>
+        <v>15.92533970044368</v>
       </c>
     </row>
     <row r="7">
@@ -545,42 +545,42 @@
         <v>24007.94921875</v>
       </c>
       <c r="C7" t="n">
-        <v>27537.849609375</v>
+        <v>27643.80078125</v>
       </c>
       <c r="D7" t="n">
-        <v>14.70304838810713</v>
+        <v>15.14436543234785</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>^CONVENTIONAL2AND3WHEELERS</t>
+          <t>MCX.NS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>64297.33</v>
+        <v>8822.8037109375</v>
       </c>
       <c r="C8" t="n">
-        <v>73496.66</v>
+        <v>10138</v>
       </c>
       <c r="D8" t="n">
-        <v>14.30748368555895</v>
+        <v>14.90678396746003</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>^FISHEXPORT</t>
+          <t>M%26M.NS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>528366.87</v>
+        <v>3177.76953125</v>
       </c>
       <c r="C9" t="n">
-        <v>603225.7</v>
+        <v>3649.39990234375</v>
       </c>
       <c r="D9" t="n">
-        <v>14.16796439186279</v>
+        <v>14.84155368901881</v>
       </c>
     </row>
     <row r="10">
@@ -590,317 +590,317 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>35793.06</v>
+        <v>35793.18</v>
       </c>
       <c r="C10" t="n">
-        <v>40693</v>
+        <v>39646.54</v>
       </c>
       <c r="D10" t="n">
-        <v>13.6896370413706</v>
+        <v>10.76562630087631</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>^DAARU</t>
+          <t>^ELECTRIC2AND3WHEELERS</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>28647.82</v>
+        <v>43136.96</v>
       </c>
       <c r="C11" t="n">
-        <v>32554.62</v>
+        <v>47581.67</v>
       </c>
       <c r="D11" t="n">
-        <v>13.63733784979101</v>
+        <v>10.30371634904268</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>^ELECTRIC2AND3WHEELERS</t>
+          <t>^DAARU</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43136.83</v>
+        <v>28646.7</v>
       </c>
       <c r="C12" t="n">
-        <v>47870.87</v>
+        <v>31394.66</v>
       </c>
       <c r="D12" t="n">
-        <v>10.97447355310996</v>
+        <v>9.592588326055004</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MCX.NS</t>
+          <t>HDFCGROWTH.NS</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8822.8037109375</v>
+        <v>119.1800003051758</v>
       </c>
       <c r="C13" t="n">
-        <v>9683</v>
+        <v>129.2100067138672</v>
       </c>
       <c r="D13" t="n">
-        <v>9.749693150218533</v>
+        <v>8.415846939929752</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HDFCGROWTH.NS</t>
+          <t>^AUTOANCILLARY</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>119.1800003051758</v>
+        <v>69440.39</v>
       </c>
       <c r="C14" t="n">
-        <v>128.0299987792969</v>
+        <v>75267.14</v>
       </c>
       <c r="D14" t="n">
-        <v>7.425741274928285</v>
+        <v>8.391009900722043</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>^AUTOANCILLARY</t>
+          <t>^FISHEXPORT</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>69440.32000000001</v>
+        <v>528366.02</v>
       </c>
       <c r="C15" t="n">
-        <v>74580.42</v>
+        <v>568029.09</v>
       </c>
       <c r="D15" t="n">
-        <v>7.402183630490168</v>
+        <v>7.506741254859642</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>^DATACENTER</t>
+          <t>^CNXMETAL</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>40447.68</v>
+        <v>9578.2001953125</v>
       </c>
       <c r="C16" t="n">
-        <v>43349.43</v>
+        <v>10265.2001953125</v>
       </c>
       <c r="D16" t="n">
-        <v>7.174082666793249</v>
+        <v>7.172537491294165</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>VAL30IETF.NS</t>
+          <t>^GOLDFINANCE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13.34000015258789</v>
+        <v>46336.23</v>
       </c>
       <c r="C17" t="n">
-        <v>14.28999996185303</v>
+        <v>49633.53</v>
       </c>
       <c r="D17" t="n">
-        <v>7.121437769105585</v>
+        <v>7.116029940286457</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>^EMS</t>
+          <t>VAL30IETF.NS</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3208.88</v>
+        <v>13.34000015258789</v>
       </c>
       <c r="C18" t="n">
-        <v>3423.67</v>
+        <v>14.14999961853027</v>
       </c>
       <c r="D18" t="n">
-        <v>6.693612724688987</v>
+        <v>6.071959945107251</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>^GOLDFINANCE</t>
+          <t>EVINDIA.NS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>46335.33</v>
+        <v>29.51000022888184</v>
       </c>
       <c r="C19" t="n">
-        <v>49338.8</v>
+        <v>31.22999954223633</v>
       </c>
       <c r="D19" t="n">
-        <v>6.482030018994148</v>
+        <v>5.828530328749729</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>EVINDIA.NS</t>
+          <t>^CNXMNC</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>29.51000022888184</v>
+        <v>28858.349609375</v>
       </c>
       <c r="C20" t="n">
-        <v>31.28000068664551</v>
+        <v>30338.55078125</v>
       </c>
       <c r="D20" t="n">
-        <v>5.997968295613052</v>
+        <v>5.129195508097032</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>^CNXMETAL</t>
+          <t>NIFTYMIDLIQ15.NS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>9578.2001953125</v>
+        <v>15622.5</v>
       </c>
       <c r="C21" t="n">
-        <v>10142.5498046875</v>
+        <v>16419.599609375</v>
       </c>
       <c r="D21" t="n">
-        <v>5.892021443143238</v>
+        <v>5.102253860617699</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>^CNXCONSUM</t>
+          <t>^CNXPHARMA</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>11870.650390625</v>
+        <v>21928.599609375</v>
       </c>
       <c r="C22" t="n">
-        <v>12500.25</v>
+        <v>22907.849609375</v>
       </c>
       <c r="D22" t="n">
-        <v>5.303834151094488</v>
+        <v>4.465629440291971</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NIFTYMIDLIQ15.NS</t>
+          <t>HDFCLOWVOL.NS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>15622.5</v>
+        <v>20.54000091552734</v>
       </c>
       <c r="C23" t="n">
-        <v>16414.75</v>
+        <v>21.39999961853027</v>
       </c>
       <c r="D23" t="n">
-        <v>5.071211393823011</v>
+        <v>4.186945787099786</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>^CNXMNC</t>
+          <t>^CNXCONSUM</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>28858.349609375</v>
+        <v>11870.650390625</v>
       </c>
       <c r="C24" t="n">
-        <v>30063.650390625</v>
+        <v>12325.2001953125</v>
       </c>
       <c r="D24" t="n">
-        <v>4.176610227420777</v>
+        <v>3.829190395890074</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>HDFCLOWVOL.NS</t>
+          <t>^ITPRODUCTS</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>20.54000091552734</v>
+        <v>60680.62</v>
       </c>
       <c r="C25" t="n">
-        <v>21.38999938964844</v>
+        <v>62826.09</v>
       </c>
       <c r="D25" t="n">
-        <v>4.13825918322395</v>
+        <v>3.535675805553724</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>^INDUSTRIALCONGLOMERATE</t>
+          <t>^EMS</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>22976.35</v>
+        <v>3208.88</v>
       </c>
       <c r="C26" t="n">
-        <v>23907.8</v>
+        <v>3319.44</v>
       </c>
       <c r="D26" t="n">
-        <v>4.053951128007716</v>
+        <v>3.445438907032981</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>^TRADINGANDBROKERAGE</t>
+          <t>HDFCQUAL.NS</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>27026.51</v>
+        <v>58.15000152587891</v>
       </c>
       <c r="C27" t="n">
-        <v>28085.1</v>
+        <v>60.09000015258789</v>
       </c>
       <c r="D27" t="n">
-        <v>3.916857929492192</v>
+        <v>3.336197034914286</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SBINEQWETF.NS</t>
+          <t>^NSEBANK</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>32.22000122070312</v>
+        <v>57443.8984375</v>
       </c>
       <c r="C28" t="n">
-        <v>33.43999862670898</v>
+        <v>59348.25</v>
       </c>
       <c r="D28" t="n">
-        <v>3.78645983794049</v>
+        <v>3.315150284537128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>^FINTECH</t>
+          <t>^HOTEL</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>85787.39</v>
+        <v>7436.37</v>
       </c>
       <c r="C29" t="n">
-        <v>88654.55</v>
+        <v>7682.38</v>
       </c>
       <c r="D29" t="n">
-        <v>3.342169519319802</v>
+        <v>3.30820010300725</v>
       </c>
     </row>
     <row r="30">
@@ -910,93 +910,93 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>40153.16</v>
+        <v>40153.14</v>
       </c>
       <c r="C30" t="n">
-        <v>41444.69</v>
+        <v>41478.73</v>
       </c>
       <c r="D30" t="n">
-        <v>3.216508987088435</v>
+        <v>3.30133583575283</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>^CNXPHARMA</t>
+          <t>SBINEQWETF.NS</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>21928.599609375</v>
+        <v>32.22000122070312</v>
       </c>
       <c r="C31" t="n">
-        <v>22580.94921875</v>
+        <v>33.22999954223633</v>
       </c>
       <c r="D31" t="n">
-        <v>2.974880389060982</v>
+        <v>3.134693616598076</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FINIETF.NS</t>
+          <t>NETFDIVOPP.NS</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>31.36000061035156</v>
+        <v>79.30999755859375</v>
       </c>
       <c r="C32" t="n">
-        <v>32.29000091552734</v>
+        <v>81.66999816894531</v>
       </c>
       <c r="D32" t="n">
-        <v>2.965562139908885</v>
+        <v>2.975665972764667</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>HDFCQUAL.NS</t>
+          <t>FINIETF.NS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>58.15000152587891</v>
+        <v>31.36000061035156</v>
       </c>
       <c r="C33" t="n">
-        <v>59.77999877929688</v>
+        <v>32.25</v>
       </c>
       <c r="D33" t="n">
-        <v>2.803090645995185</v>
+        <v>2.838008202572099</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>INFRABEES.NS</t>
+          <t>^FINTECH</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>972.260009765625</v>
+        <v>85788.14</v>
       </c>
       <c r="C34" t="n">
-        <v>998.3400268554688</v>
+        <v>88172.56</v>
       </c>
       <c r="D34" t="n">
-        <v>2.682411785724958</v>
+        <v>2.77942848510295</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>^NIFTYEV&amp;NEWAGEAUTOMOTIVE</t>
+          <t>^ONLINEPLATFORM</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>28689.55</v>
+        <v>57439.06</v>
       </c>
       <c r="C35" t="n">
-        <v>29450.73</v>
+        <v>58998.46</v>
       </c>
       <c r="D35" t="n">
-        <v>2.653161168439381</v>
+        <v>2.714877297783079</v>
       </c>
     </row>
     <row r="36">
@@ -1009,170 +1009,170 @@
         <v>16760.94921875</v>
       </c>
       <c r="C36" t="n">
-        <v>17204.349609375</v>
+        <v>17215.349609375</v>
       </c>
       <c r="D36" t="n">
-        <v>2.645437229348446</v>
+        <v>2.711065970635333</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>^NSEBANK</t>
+          <t>^TRADINGANDBROKERAGE</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>57443.8984375</v>
+        <v>27026.27</v>
       </c>
       <c r="C37" t="n">
-        <v>58867.69921875</v>
+        <v>27755.81</v>
       </c>
       <c r="D37" t="n">
-        <v>2.478593584310997</v>
+        <v>2.699373609454804</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NETFDIVOPP.NS</t>
+          <t>^INDUSTRIALCONGLOMERATE</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>79.30999755859375</v>
+        <v>22976.34</v>
       </c>
       <c r="C38" t="n">
-        <v>81.26000213623047</v>
+        <v>23582.97</v>
       </c>
       <c r="D38" t="n">
-        <v>2.458712189716141</v>
+        <v>2.640237740214503</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BSLNIFTY.NS</t>
+          <t>SDL26BEES.NS</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>29.55999946594238</v>
+        <v>131.6900024414062</v>
       </c>
       <c r="C39" t="n">
-        <v>30.27000045776367</v>
+        <v>134.7899932861328</v>
       </c>
       <c r="D39" t="n">
-        <v>2.401897850638726</v>
+        <v>2.354006217067133</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>^HOTEL</t>
+          <t>BSLNIFTY.NS</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>7436.37</v>
+        <v>29.55999946594238</v>
       </c>
       <c r="C40" t="n">
-        <v>7613.37</v>
+        <v>30.25</v>
       </c>
       <c r="D40" t="n">
-        <v>2.380193562181549</v>
+        <v>2.334237302177907</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>^CNXINFRA</t>
+          <t>^NIFTYEV&amp;NEWAGEAUTOMOTIVE</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>9438.7001953125</v>
+        <v>28689.64</v>
       </c>
       <c r="C41" t="n">
-        <v>9661.4501953125</v>
+        <v>29271.71</v>
       </c>
       <c r="D41" t="n">
-        <v>2.35996477683043</v>
+        <v>2.028850832565343</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>^ONLINEPLATFORM</t>
+          <t>NIFTYBEES.NS</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>57440.71</v>
+        <v>287.9599914550781</v>
       </c>
       <c r="C42" t="n">
-        <v>58721.63</v>
+        <v>293.7999877929688</v>
       </c>
       <c r="D42" t="n">
-        <v>2.229986363330116</v>
+        <v>2.028058241139956</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>NIFTYBEES.NS</t>
+          <t>NV20.NS</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>287.9599914550781</v>
+        <v>150.7200012207031</v>
       </c>
       <c r="C43" t="n">
-        <v>294.3200073242188</v>
+        <v>153.7400054931641</v>
       </c>
       <c r="D43" t="n">
-        <v>2.208645665324237</v>
+        <v>2.003718317410752</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>^ITPRODUCTS</t>
+          <t>^CNXCMDT</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>60680.55</v>
+        <v>8974.7998046875</v>
       </c>
       <c r="C44" t="n">
-        <v>62016.94</v>
+        <v>9136.599609375</v>
       </c>
       <c r="D44" t="n">
-        <v>2.202336663065841</v>
+        <v>1.802823552710253</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>^CNXCMDT</t>
+          <t>NIFTY_MIDCAP_100.NS</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>8974.7998046875</v>
+        <v>59385.1484375</v>
       </c>
       <c r="C45" t="n">
-        <v>9172</v>
+        <v>60315.6484375</v>
       </c>
       <c r="D45" t="n">
-        <v>2.197265672817606</v>
+        <v>1.56689008023497</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SDL26BEES.NS</t>
+          <t>^DATACENTER</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>131.6900024414062</v>
+        <v>40446.52</v>
       </c>
       <c r="C46" t="n">
-        <v>134.2400054931641</v>
+        <v>41019.4</v>
       </c>
       <c r="D46" t="n">
-        <v>1.936367988824667</v>
+        <v>1.416388851253469</v>
       </c>
     </row>
     <row r="47">
@@ -1185,218 +1185,218 @@
         <v>25637.80078125</v>
       </c>
       <c r="C47" t="n">
-        <v>26068.150390625</v>
+        <v>25986</v>
       </c>
       <c r="D47" t="n">
-        <v>1.678574590101865</v>
+        <v>1.35814776673299</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>^HOSPITAL</t>
+          <t>NIFTYMIDCAP150.NS</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>20020.31</v>
+        <v>21840.19921875</v>
       </c>
       <c r="C48" t="n">
-        <v>20336.59</v>
+        <v>22130.150390625</v>
       </c>
       <c r="D48" t="n">
-        <v>1.579795717448925</v>
+        <v>1.32760314579033</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>NIFTY_MIDCAP_100.NS</t>
+          <t>^CNX200</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>59385.1484375</v>
+        <v>14276.0498046875</v>
       </c>
       <c r="C49" t="n">
-        <v>60276.30078125</v>
+        <v>14444.400390625</v>
       </c>
       <c r="D49" t="n">
-        <v>1.50063166835037</v>
+        <v>1.179251881582975</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>^CNX200</t>
+          <t>ICICIQTY30.NS</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>14276.0498046875</v>
+        <v>21.60000038146973</v>
       </c>
       <c r="C50" t="n">
-        <v>14481.5</v>
+        <v>21.85000038146973</v>
       </c>
       <c r="D50" t="n">
-        <v>1.439124954895023</v>
+        <v>1.157407386966857</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NIFTYMIDCAP150.NS</t>
+          <t>^CNX100</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>21840.19921875</v>
+        <v>26223.599609375</v>
       </c>
       <c r="C51" t="n">
-        <v>22151.150390625</v>
+        <v>26506.099609375</v>
       </c>
       <c r="D51" t="n">
-        <v>1.423756114862019</v>
+        <v>1.077273921994315</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>^CNX100</t>
+          <t>INFRABEES.NS</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>26223.599609375</v>
+        <v>972.260009765625</v>
       </c>
       <c r="C52" t="n">
-        <v>26593.19921875</v>
+        <v>982.6300048828125</v>
       </c>
       <c r="D52" t="n">
-        <v>1.40941600268663</v>
+        <v>1.066586613974518</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>NV20.NS</t>
+          <t>NIFTY_FIN_SERVICE.NS</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>150.7200012207031</v>
+        <v>27344.05078125</v>
       </c>
       <c r="C53" t="n">
-        <v>152.7200012207031</v>
+        <v>27629.599609375</v>
       </c>
       <c r="D53" t="n">
-        <v>1.326963895834468</v>
+        <v>1.044281370047786</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ICICIQTY30.NS</t>
+          <t>^CNXINFRA</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>21.60000038146973</v>
+        <v>9438.7001953125</v>
       </c>
       <c r="C54" t="n">
-        <v>21.8700008392334</v>
+        <v>9509.5</v>
       </c>
       <c r="D54" t="n">
-        <v>1.250002097200427</v>
+        <v>0.7501012133287271</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ECAPINSURE.NS</t>
+          <t>^HOSPITAL</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>23.82999992370605</v>
+        <v>20020.28</v>
       </c>
       <c r="C55" t="n">
-        <v>24.07999992370605</v>
+        <v>20110.93</v>
       </c>
       <c r="D55" t="n">
-        <v>1.049097779271498</v>
+        <v>0.4527908700577687</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>NIFTY_FIN_SERVICE.NS</t>
+          <t>^CRSLDX</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>27344.05078125</v>
+        <v>23620.150390625</v>
       </c>
       <c r="C56" t="n">
-        <v>27566.150390625</v>
+        <v>23716.30078125</v>
       </c>
       <c r="D56" t="n">
-        <v>0.8122410653482811</v>
+        <v>0.4070693413669489</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>^CRSLDX</t>
+          <t>TOP10ADD.NS</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>23620.150390625</v>
+        <v>100.9400024414062</v>
       </c>
       <c r="C57" t="n">
-        <v>23790.25</v>
+        <v>101.2200012207031</v>
       </c>
       <c r="D57" t="n">
-        <v>0.7201461741857228</v>
+        <v>0.2773912943576646</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>^CNXFMCG</t>
+          <t>ECAPINSURE.NS</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>55109</v>
+        <v>23.82999992370605</v>
       </c>
       <c r="C58" t="n">
-        <v>55504.69921875</v>
+        <v>23.86000061035156</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7180301198533814</v>
+        <v>0.1258946149456894</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>^SEMICONDUCTOR</t>
+          <t>^PAINT</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>31177</v>
+        <v>14498.25</v>
       </c>
       <c r="C59" t="n">
-        <v>31355.59</v>
+        <v>14505.37</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5728261218205734</v>
+        <v>0.0491093752694346</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>^PAINT</t>
+          <t>MAESGETF.NS</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>14498.29</v>
+        <v>41.0099983215332</v>
       </c>
       <c r="C60" t="n">
-        <v>14557.25</v>
+        <v>41.0099983215332</v>
       </c>
       <c r="D60" t="n">
-        <v>0.4066686485095768</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1409,298 +1409,298 @@
         <v>16.5</v>
       </c>
       <c r="C61" t="n">
-        <v>16.55999946594238</v>
+        <v>16.48999977111816</v>
       </c>
       <c r="D61" t="n">
-        <v>0.3636331269235322</v>
+        <v>-0.06060744776870265</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>TOP10ADD.NS</t>
+          <t>^CNXSERVICE</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>100.9400024414062</v>
+        <v>33875.05078125</v>
       </c>
       <c r="C62" t="n">
-        <v>100.9499969482422</v>
+        <v>33777.3515625</v>
       </c>
       <c r="D62" t="n">
-        <v>0.009901433122848515</v>
+        <v>-0.2884105455100217</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>MAESGETF.NS</t>
+          <t>^CNXFMCG</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>41.0099983215332</v>
+        <v>55109</v>
       </c>
       <c r="C63" t="n">
-        <v>41.0099983215332</v>
+        <v>54949.1015625</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>-0.2901494084450816</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>^NSMIDCP</t>
+          <t>HDFCBANK.NS</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>68712.3984375</v>
+        <v>1004.949157714844</v>
       </c>
       <c r="C64" t="n">
-        <v>68669.1484375</v>
+        <v>1000.5</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.06294351672113395</v>
+        <v>-0.4427246573309938</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>^CNXSERVICE</t>
+          <t>^NSMIDCP</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>33875.05078125</v>
+        <v>68712.3984375</v>
       </c>
       <c r="C65" t="n">
-        <v>33809.30078125</v>
+        <v>68400.8515625</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.1940956499949896</v>
+        <v>-0.4534070736642666</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>HDFCBANK.NS</t>
+          <t>SHARIABEES.NS</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1004.949157714844</v>
+        <v>514.9600219726562</v>
       </c>
       <c r="C66" t="n">
-        <v>998.0499877929688</v>
+        <v>512.219970703125</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.6865192998980206</v>
+        <v>-0.5320900948844419</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SHARIABEES.NS</t>
+          <t>ICICIALPLV.NS</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>514.9600219726562</v>
+        <v>28</v>
       </c>
       <c r="C67" t="n">
-        <v>510.1199951171875</v>
+        <v>27.84000015258789</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.9398840004954306</v>
+        <v>-0.5714280264718192</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ICICIALPLV.NS</t>
+          <t>ALPHAETF.NS</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>28</v>
+        <v>25.86000061035156</v>
       </c>
       <c r="C68" t="n">
-        <v>27.72999954223633</v>
+        <v>25.47999954223633</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.9642873491559709</v>
+        <v>-1.469454985098194</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ALPHAETF.NS</t>
+          <t>^SEMICONDUCTOR</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>25.86000061035156</v>
+        <v>31177.2</v>
       </c>
       <c r="C69" t="n">
-        <v>25.57999992370605</v>
+        <v>30519.02</v>
       </c>
       <c r="D69" t="n">
-        <v>-1.082755916615971</v>
+        <v>-2.111094004593101</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>^INSURANCE</t>
+          <t>^CNXIT</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>7379.19</v>
+        <v>38822.94921875</v>
       </c>
       <c r="C70" t="n">
-        <v>7267.71</v>
+        <v>37825.25</v>
       </c>
       <c r="D70" t="n">
-        <v>-1.510734918060106</v>
+        <v>-2.569869726095279</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>^CNXENERGY</t>
+          <t>^INSURANCE</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>36542.6015625</v>
+        <v>7379.7</v>
       </c>
       <c r="C71" t="n">
-        <v>35852.3984375</v>
+        <v>7157.13</v>
       </c>
       <c r="D71" t="n">
-        <v>-1.888762965656737</v>
+        <v>-3.015976259197525</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>^CNXPSE</t>
+          <t>MIDQ50ADD.NS</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>10078.099609375</v>
+        <v>255.1999969482422</v>
       </c>
       <c r="C72" t="n">
-        <v>9867.0498046875</v>
+        <v>247.2400054931641</v>
       </c>
       <c r="D72" t="n">
-        <v>-2.094142872840571</v>
+        <v>-3.119118946029029</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>^SHIPBUILDINGANDSERVICING</t>
+          <t>^WOODPRODUCTS</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>15769.37</v>
+        <v>99189.67999999999</v>
       </c>
       <c r="C73" t="n">
-        <v>15435.14</v>
+        <v>96062.73</v>
       </c>
       <c r="D73" t="n">
-        <v>-2.119488603539655</v>
+        <v>-3.152495299914262</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MOMENTUM50.NS</t>
+          <t>^TRAVEL</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>55.43999862670898</v>
+        <v>12055.64</v>
       </c>
       <c r="C74" t="n">
-        <v>54.16999816894531</v>
+        <v>11618.29</v>
       </c>
       <c r="D74" t="n">
-        <v>-2.29076567320085</v>
+        <v>-3.627762607377116</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>EMULTIMQ.NS</t>
+          <t>MOMENTUM50.NS</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>43.83000183105469</v>
+        <v>55.43999862670898</v>
       </c>
       <c r="C75" t="n">
-        <v>42.81000137329102</v>
+        <v>53.31000137329102</v>
       </c>
       <c r="D75" t="n">
-        <v>-2.327174116248782</v>
+        <v>-3.841986483007979</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MIDQ50ADD.NS</t>
+          <t>EMULTIMQ.NS</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>255.1999969482422</v>
+        <v>43.83000183105469</v>
       </c>
       <c r="C76" t="n">
-        <v>248.8099975585938</v>
+        <v>42.11999893188477</v>
       </c>
       <c r="D76" t="n">
-        <v>-2.503918286074435</v>
+        <v>-3.901443823254283</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>^TRAVEL</t>
+          <t>^CNXENERGY</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>12055.79</v>
+        <v>36542.6015625</v>
       </c>
       <c r="C77" t="n">
-        <v>11718.88</v>
+        <v>35105</v>
       </c>
       <c r="D77" t="n">
-        <v>-2.794590814869881</v>
+        <v>-3.934042736506385</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>^WOODPRODUCTS</t>
+          <t>ALPHA.NS</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>99191.50999999999</v>
+        <v>51.47000122070312</v>
       </c>
       <c r="C78" t="n">
-        <v>96095.61</v>
+        <v>49.31999969482422</v>
       </c>
       <c r="D78" t="n">
-        <v>-3.121134056735293</v>
+        <v>-4.177193461992957</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>^DELIVERY</t>
+          <t>^CNXPSE</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>8138.96</v>
+        <v>10078.099609375</v>
       </c>
       <c r="C79" t="n">
-        <v>7877.59</v>
+        <v>9616.75</v>
       </c>
       <c r="D79" t="n">
-        <v>-3.211343955493084</v>
+        <v>-4.577744091215734</v>
       </c>
     </row>
     <row r="80">
@@ -1713,218 +1713,218 @@
         <v>51.11999893188477</v>
       </c>
       <c r="C80" t="n">
-        <v>49.18000030517578</v>
+        <v>48.68000030517578</v>
       </c>
       <c r="D80" t="n">
-        <v>-3.794989568160888</v>
+        <v>-4.773080355420546</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ALPHA.NS</t>
+          <t>^DELIVERY</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>51.47000122070312</v>
+        <v>8139.59</v>
       </c>
       <c r="C81" t="n">
-        <v>49.41999816894531</v>
+        <v>7684.14</v>
       </c>
       <c r="D81" t="n">
-        <v>-3.982908496480132</v>
+        <v>-5.595490681963094</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>^CHEMICAL</t>
+          <t>^CONVENTIONALPOWER</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>55602.92</v>
+        <v>6267.88</v>
       </c>
       <c r="C82" t="n">
-        <v>53309.48</v>
+        <v>5899.78</v>
       </c>
       <c r="D82" t="n">
-        <v>-4.124675466684115</v>
+        <v>-5.872799096345181</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>^CONVENTIONALPOWER</t>
+          <t>^SHIPBUILDINGANDSERVICING</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>6268.12</v>
+        <v>15769.47</v>
       </c>
       <c r="C83" t="n">
-        <v>5988.12</v>
+        <v>14725.13</v>
       </c>
       <c r="D83" t="n">
-        <v>-4.467049131158944</v>
+        <v>-6.622543433609374</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>^CNXIT</t>
+          <t>^CHEMICAL</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>38822.94921875</v>
+        <v>55603.31</v>
       </c>
       <c r="C84" t="n">
-        <v>36885.3515625</v>
+        <v>51633.95</v>
       </c>
       <c r="D84" t="n">
-        <v>-4.990856427038816</v>
+        <v>-7.138711706191593</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>^CEMENT</t>
+          <t>^WIREANDCABLE</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>10664.49</v>
+        <v>63171.74</v>
       </c>
       <c r="C85" t="n">
-        <v>10075.25</v>
+        <v>58490.59</v>
       </c>
       <c r="D85" t="n">
-        <v>-5.525252496837634</v>
+        <v>-7.410196394780328</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>^WIREANDCABLE</t>
+          <t>^CEMENT</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>63171.11</v>
+        <v>10664.49</v>
       </c>
       <c r="C86" t="n">
-        <v>59395.21</v>
+        <v>9844.870000000001</v>
       </c>
       <c r="D86" t="n">
-        <v>-5.977257641982231</v>
+        <v>-7.685505823532106</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>^RENEWABLEPOWER</t>
+          <t>SMALLCAP.NS</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>6201.6</v>
+        <v>48.34000015258789</v>
       </c>
       <c r="C87" t="n">
-        <v>5776.95</v>
+        <v>44.29000091552734</v>
       </c>
       <c r="D87" t="n">
-        <v>-6.847426470588244</v>
+        <v>-8.378153132553786</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>SMALLCAP.NS</t>
+          <t>^SOLARMANUFACTURINGANDMAINTENANCE</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>48.34000015258789</v>
+        <v>11066.21</v>
       </c>
       <c r="C88" t="n">
-        <v>44.90000152587891</v>
+        <v>10094.29</v>
       </c>
       <c r="D88" t="n">
-        <v>-7.116256962868096</v>
+        <v>-8.782772060172347</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>^ELECTRONICAPPLIANCE</t>
+          <t>^TELECOMSERVICE</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>32247.18</v>
+        <v>9820.719999999999</v>
       </c>
       <c r="C89" t="n">
-        <v>29889.74</v>
+        <v>8958.15</v>
       </c>
       <c r="D89" t="n">
-        <v>-7.310530719275294</v>
+        <v>-8.783164574491481</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>MODEFENCE.NS</t>
+          <t>^ELECTRONICAPPLIANCE</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>96.36000061035156</v>
+        <v>32247.17</v>
       </c>
       <c r="C90" t="n">
-        <v>89.13999938964844</v>
+        <v>29080.43</v>
       </c>
       <c r="D90" t="n">
-        <v>-7.492736794282989</v>
+        <v>-9.820210579719083</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>^SOLARMANUFACTURINGANDMAINTENANCE</t>
+          <t>^RENEWABLEPOWER</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>11066.21</v>
+        <v>6201.6</v>
       </c>
       <c r="C91" t="n">
-        <v>10236.58</v>
+        <v>5580.51</v>
       </c>
       <c r="D91" t="n">
-        <v>-7.496965989259189</v>
+        <v>-10.01499613003096</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>^TRANSFORMERMANUFACTURERS</t>
+          <t>^PORTSOPERATION</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>17110.91</v>
+        <v>9877.67</v>
       </c>
       <c r="C92" t="n">
-        <v>15773.1</v>
+        <v>8884.799999999999</v>
       </c>
       <c r="D92" t="n">
-        <v>-7.818462022183505</v>
+        <v>-10.05166198101375</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>^TELECOMSERVICE</t>
+          <t>^IRONPIPE</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>9820.74</v>
+        <v>32658.59</v>
       </c>
       <c r="C93" t="n">
-        <v>9036.6</v>
+        <v>29097.31</v>
       </c>
       <c r="D93" t="n">
-        <v>-7.984530697279426</v>
+        <v>-10.90457365122009</v>
       </c>
     </row>
     <row r="94">
@@ -1937,58 +1937,58 @@
         <v>993.9500122070312</v>
       </c>
       <c r="C94" t="n">
-        <v>905.5999755859375</v>
+        <v>885.3499755859375</v>
       </c>
       <c r="D94" t="n">
-        <v>-8.888780676697774</v>
+        <v>-10.92610647289507</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>^ELECTRONICDEFENCE</t>
+          <t>^TRANSFORMERMANUFACTURERS</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>63762.96</v>
+        <v>17112.98</v>
       </c>
       <c r="C95" t="n">
-        <v>58009.98</v>
+        <v>15236.9</v>
       </c>
       <c r="D95" t="n">
-        <v>-9.022448142307063</v>
+        <v>-10.96290651891138</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>^PORTSOPERATION</t>
+          <t>MODEFENCE.NS</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>9877.540000000001</v>
+        <v>96.36000061035156</v>
       </c>
       <c r="C96" t="n">
-        <v>8981.790000000001</v>
+        <v>85.79000091552734</v>
       </c>
       <c r="D96" t="n">
-        <v>-9.068553506237382</v>
+        <v>-10.96928147350876</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>^IRONPIPE</t>
+          <t>^ELECTRONICDEFENCE</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>32658.93</v>
+        <v>63766.91</v>
       </c>
       <c r="C97" t="n">
-        <v>29130.51</v>
+        <v>55756</v>
       </c>
       <c r="D97" t="n">
-        <v>-10.80384446153013</v>
+        <v>-12.56280098878871</v>
       </c>
     </row>
     <row r="98">
@@ -1998,109 +1998,109 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>58182.54</v>
+        <v>58181.51</v>
       </c>
       <c r="C98" t="n">
-        <v>51562.58</v>
+        <v>50869.66</v>
       </c>
       <c r="D98" t="n">
-        <v>-11.37791509274088</v>
+        <v>-12.56730875496356</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>^TEXTILESANDAPPARELS</t>
+          <t>^AGRICULTURE</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>55916.25</v>
+        <v>34268.88</v>
       </c>
       <c r="C99" t="n">
-        <v>49493.85</v>
+        <v>29645.26</v>
       </c>
       <c r="D99" t="n">
-        <v>-11.48574877607136</v>
+        <v>-13.49218299518397</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>^HOUSINGFINANCE</t>
+          <t>^TELECOMEQUIPMENTSANDACCESSORIES</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>8015.26</v>
+        <v>27771.66</v>
       </c>
       <c r="C100" t="n">
-        <v>7089.03</v>
+        <v>23872</v>
       </c>
       <c r="D100" t="n">
-        <v>-11.55583224998316</v>
+        <v>-14.04186858113631</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>^AGRICULTURE</t>
+          <t>^TEXTILESANDAPPARELS</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>34268.84</v>
+        <v>55916.21</v>
       </c>
       <c r="C101" t="n">
-        <v>29925.4</v>
+        <v>47965.07</v>
       </c>
       <c r="D101" t="n">
-        <v>-12.67460468460559</v>
+        <v>-14.21974057254596</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>^TELECOMEQUIPMENTSANDACCESSORIES</t>
+          <t>^HOUSINGFINANCE</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>27771.66</v>
+        <v>8015.24</v>
       </c>
       <c r="C102" t="n">
-        <v>24035.16</v>
+        <v>6788.32</v>
       </c>
       <c r="D102" t="n">
-        <v>-13.45436318894873</v>
+        <v>-15.3073395182178</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>^PLASTICPIPE</t>
+          <t>^CNXMEDIA</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>61384.89</v>
+        <v>1747.849975585938</v>
       </c>
       <c r="C103" t="n">
-        <v>51978.08</v>
+        <v>1462.550048828125</v>
       </c>
       <c r="D103" t="n">
-        <v>-15.32430863686487</v>
+        <v>-16.32290704253209</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>^CNXMEDIA</t>
+          <t>^PLASTICPIPE</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>1747.849975585938</v>
+        <v>61384.38</v>
       </c>
       <c r="C104" t="n">
-        <v>1444.199951171875</v>
+        <v>49778.19</v>
       </c>
       <c r="D104" t="n">
-        <v>-17.37277390253525</v>
+        <v>-18.90739956972767</v>
       </c>
     </row>
     <row r="105">
@@ -2113,10 +2113,10 @@
         <v>82.19999694824219</v>
       </c>
       <c r="C105" t="n">
-        <v>52.15000152587891</v>
+        <v>53.20000076293945</v>
       </c>
       <c r="D105" t="n">
-        <v>-36.55717340389255</v>
+        <v>-35.27980202184531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>